<commit_message>
chuyen file bien ban cuoc hop sang 00.
</commit_message>
<xml_diff>
--- a/00. Project Management/ProjectPlan.xlsx
+++ b/00. Project Management/ProjectPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
   <si>
     <t>KẾ HOẠCH DỰ ÁN</t>
   </si>
@@ -174,6 +174,51 @@
   </si>
   <si>
     <t>15/8/2023</t>
+  </si>
+  <si>
+    <t>1.4.1.1</t>
+  </si>
+  <si>
+    <t>Thiết kế Landing Page</t>
+  </si>
+  <si>
+    <t>16/8/2023</t>
+  </si>
+  <si>
+    <t>17/8/2023</t>
+  </si>
+  <si>
+    <t>1.4.1.2</t>
+  </si>
+  <si>
+    <t>Thiết kế form Đăng nhập, Đăng ký</t>
+  </si>
+  <si>
+    <t>1.4.2.1</t>
+  </si>
+  <si>
+    <t>Dựng model và ánh xạ CSDL</t>
+  </si>
+  <si>
+    <t>1.4.2.2</t>
+  </si>
+  <si>
+    <t>Trạng</t>
+  </si>
+  <si>
+    <t>Dựng phần upload ảnh qua API và mock data</t>
+  </si>
+  <si>
+    <t>1.4.2.3</t>
+  </si>
+  <si>
+    <t>Cấu hình bảo mật và dựng các Controller cho tất cả các Model</t>
+  </si>
+  <si>
+    <t>Dựng phần đăng nhập, đăng ký</t>
+  </si>
+  <si>
+    <t>1.4.2.4</t>
   </si>
 </sst>
 </file>
@@ -891,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,8 +1362,12 @@
       <c r="F16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="I16" s="11"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1342,7 +1391,9 @@
       <c r="F17" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="H17" s="13"/>
       <c r="I17" s="11"/>
       <c r="J17" s="13"/>
@@ -1390,24 +1441,24 @@
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D20" s="11">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
@@ -1415,124 +1466,196 @@
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="53.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="11">
+        <v>1</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+    </row>
+    <row r="22" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="11">
+        <v>8</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" ht="53.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="11">
+        <v>1</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" ht="70.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="11">
+        <v>1</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+    </row>
+    <row r="28" spans="1:11" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="11">
+        <v>1</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+    </row>
+    <row r="29" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="15"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="18"/>
       <c r="C30" s="8"/>
@@ -1557,6 +1680,58 @@
       <c r="I31" s="8"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>